<commit_message>
Some New Models Trained
</commit_message>
<xml_diff>
--- a/src/cnns/overall_results.xlsx
+++ b/src/cnns/overall_results.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:P41"/>
+  <dimension ref="A1:P43"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -3027,6 +3027,138 @@
         <v>1692.633374929428</v>
       </c>
     </row>
+    <row r="42">
+      <c r="A42" t="inlineStr">
+        <is>
+          <t>InceptionResNetV2_10</t>
+        </is>
+      </c>
+      <c r="B42" t="inlineStr">
+        <is>
+          <t>InceptionResNetV2</t>
+        </is>
+      </c>
+      <c r="C42" t="n">
+        <v>0.9678391959798995</v>
+      </c>
+      <c r="D42" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="E42" t="n">
+        <v>7</v>
+      </c>
+      <c r="F42" t="inlineStr">
+        <is>
+          <t>['Functional', 'Dropout', 'BatchNormalization', 'Dense', 'Dropout', 'BatchNormalization', 'Dense']</t>
+        </is>
+      </c>
+      <c r="G42" t="inlineStr">
+        <is>
+          <t>[0.1, 0.1]</t>
+        </is>
+      </c>
+      <c r="H42" t="inlineStr">
+        <is>
+          <t>[('relu', 1024), ('softmax', 15)]</t>
+        </is>
+      </c>
+      <c r="I42" t="n">
+        <v>70</v>
+      </c>
+      <c r="J42" t="n">
+        <v>0.0001</v>
+      </c>
+      <c r="K42" t="inlineStr">
+        <is>
+          <t>{'monitor': 'val_loss', 'patience': 15, 'min_delta': 0, 'restore_best_weights': True}</t>
+        </is>
+      </c>
+      <c r="L42" t="inlineStr">
+        <is>
+          <t>{'Train': 32, 'Validation': 32}</t>
+        </is>
+      </c>
+      <c r="M42" t="inlineStr">
+        <is>
+          <t>{'zoom_range': 0.2, 'rotation_range': 30, 'shear_range': 0.2, 'brightness_range': None, 'horizontal_flip': True, 'width_shift_range': 0.2, 'height_shift_range': 0.2}</t>
+        </is>
+      </c>
+      <c r="N42" t="n">
+        <v>55936239</v>
+      </c>
+      <c r="O42" t="n">
+        <v>0</v>
+      </c>
+      <c r="P42" t="n">
+        <v>2777.928627490997</v>
+      </c>
+    </row>
+    <row r="43">
+      <c r="A43" t="inlineStr">
+        <is>
+          <t>InceptionResNetV2_18</t>
+        </is>
+      </c>
+      <c r="B43" t="inlineStr">
+        <is>
+          <t>InceptionResNetV2</t>
+        </is>
+      </c>
+      <c r="C43" t="n">
+        <v>0.9447236180904522</v>
+      </c>
+      <c r="D43" t="n">
+        <v>0.9166666666666666</v>
+      </c>
+      <c r="E43" t="n">
+        <v>7</v>
+      </c>
+      <c r="F43" t="inlineStr">
+        <is>
+          <t>['Functional', 'Dropout', 'BatchNormalization', 'Dense', 'Dropout', 'BatchNormalization', 'Dense']</t>
+        </is>
+      </c>
+      <c r="G43" t="inlineStr">
+        <is>
+          <t>[0.1, 0.1]</t>
+        </is>
+      </c>
+      <c r="H43" t="inlineStr">
+        <is>
+          <t>[('relu', 1024), ('softmax', 15)]</t>
+        </is>
+      </c>
+      <c r="I43" t="n">
+        <v>70</v>
+      </c>
+      <c r="J43" t="n">
+        <v>1e-05</v>
+      </c>
+      <c r="K43" t="inlineStr">
+        <is>
+          <t>{'monitor': 'val_loss', 'patience': 15, 'min_delta': 0, 'restore_best_weights': True}</t>
+        </is>
+      </c>
+      <c r="L43" t="inlineStr">
+        <is>
+          <t>{'Train': 32, 'Validation': 32}</t>
+        </is>
+      </c>
+      <c r="M43" t="inlineStr">
+        <is>
+          <t>{'zoom_range': 0.2, 'rotation_range': 30, 'shear_range': 0.2, 'brightness_range': None, 'horizontal_flip': True, 'width_shift_range': 0.2, 'height_shift_range': 0.2}</t>
+        </is>
+      </c>
+      <c r="N43" t="n">
+        <v>55936239</v>
+      </c>
+      <c r="O43" t="n">
+        <v>0</v>
+      </c>
+      <c r="P43" t="n">
+        <v>3645.254849910736</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
 </worksheet>

</xml_diff>

<commit_message>
Last Model CNN Added
</commit_message>
<xml_diff>
--- a/src/cnns/overall_results.xlsx
+++ b/src/cnns/overall_results.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Diego\CACHARREANDOPY\ICAI\ML2\DeepLearning\practica_final\ml2-deep-learning\src\cnns\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{30B69BBC-E8D3-420A-A972-212AED4353DF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{084B2810-3114-4112-BEEC-F25D60D6AD01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="328" uniqueCount="109">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="344" uniqueCount="113">
   <si>
     <t>Model</t>
   </si>
@@ -304,42 +304,42 @@
     <t>{'Train': 64, 'Validation': 64}</t>
   </si>
   <si>
+    <t>InceptionResNetV2_11</t>
+  </si>
+  <si>
+    <t>['Functional', 'Dropout', 'BatchNormalization', 'Dense', 'Dropout', 'BatchNormalization', 'Dense']</t>
+  </si>
+  <si>
+    <t>[('relu', 4096), ('softmax', 15)]</t>
+  </si>
+  <si>
+    <t>{'monitor': 'val_loss', 'patience': 20, 'min_delta': 0, 'restore_best_weights': True}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_13</t>
+  </si>
+  <si>
+    <t>{'zoom_range': 0.4, 'rotation_range': 40, 'shear_range': 0.4, 'brightness_range': (0.2, 0.8), 'horizontal_flip': True, 'width_shift_range': 0.3, 'height_shift_range': 0.3}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_14</t>
+  </si>
+  <si>
+    <t>{'zoom_range': [0.5, 1.5], 'rotation_range': 90, 'shear_range': 45.0, 'brightness_range': (0.2, 0.8), 'horizontal_flip': True, 'width_shift_range': 0.4, 'height_shift_range': 0.3}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_15</t>
+  </si>
+  <si>
+    <t>{'zoom_range': [0.3, 1.8], 'rotation_range': 70, 'shear_range': 45.0, 'brightness_range': (0.3, 0.75), 'horizontal_flip': True, 'width_shift_range': 0.5, 'height_shift_range': 0.5}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_16</t>
+  </si>
+  <si>
     <t>InceptionResNetV2_10</t>
   </si>
   <si>
-    <t>['Functional', 'Dropout', 'BatchNormalization', 'Dense', 'Dropout', 'BatchNormalization', 'Dense']</t>
-  </si>
-  <si>
-    <t>InceptionResNetV2_11</t>
-  </si>
-  <si>
-    <t>[('relu', 4096), ('softmax', 15)]</t>
-  </si>
-  <si>
-    <t>{'monitor': 'val_loss', 'patience': 20, 'min_delta': 0, 'restore_best_weights': True}</t>
-  </si>
-  <si>
-    <t>InceptionResNetV2_13</t>
-  </si>
-  <si>
-    <t>{'zoom_range': 0.4, 'rotation_range': 40, 'shear_range': 0.4, 'brightness_range': (0.2, 0.8), 'horizontal_flip': True, 'width_shift_range': 0.3, 'height_shift_range': 0.3}</t>
-  </si>
-  <si>
-    <t>InceptionResNetV2_14</t>
-  </si>
-  <si>
-    <t>{'zoom_range': [0.5, 1.5], 'rotation_range': 90, 'shear_range': 45.0, 'brightness_range': (0.2, 0.8), 'horizontal_flip': True, 'width_shift_range': 0.4, 'height_shift_range': 0.3}</t>
-  </si>
-  <si>
-    <t>InceptionResNetV2_15</t>
-  </si>
-  <si>
-    <t>{'zoom_range': [0.3, 1.8], 'rotation_range': 70, 'shear_range': 45.0, 'brightness_range': (0.3, 0.75), 'horizontal_flip': True, 'width_shift_range': 0.5, 'height_shift_range': 0.5}</t>
-  </si>
-  <si>
-    <t>InceptionResNetV2_16</t>
-  </si>
-  <si>
     <t>InceptionResNetV2_18</t>
   </si>
   <si>
@@ -347,6 +347,18 @@
   </si>
   <si>
     <t>{'Train': 128, 'Validation': 128}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_19</t>
+  </si>
+  <si>
+    <t>{'monitor': 'val_loss', 'patience': 30, 'min_delta': 0, 'restore_best_weights': True}</t>
+  </si>
+  <si>
+    <t>InceptionResNetV2_20</t>
+  </si>
+  <si>
+    <t>{'monitor': 'val_loss', 'patience': 25, 'min_delta': 0, 'restore_best_weights': True}</t>
   </si>
 </sst>
 </file>
@@ -709,15 +721,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P44"/>
+  <dimension ref="A1:P46"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A18" workbookViewId="0">
-      <selection activeCell="A31" sqref="A31"/>
-    </sheetView>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="32.5546875" customWidth="1"/>
+    <col min="1" max="1" width="46.21875" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.3">
@@ -2376,7 +2386,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="B36" t="s">
         <v>34</v>
@@ -2397,7 +2407,7 @@
         <v>61</v>
       </c>
       <c r="H36" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I36">
         <v>70</v>
@@ -2406,7 +2416,7 @@
         <v>1E-4</v>
       </c>
       <c r="K36" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L36" t="s">
         <v>22</v>
@@ -2426,7 +2436,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="B37" t="s">
         <v>34</v>
@@ -2447,7 +2457,7 @@
         <v>61</v>
       </c>
       <c r="H37" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="I37">
         <v>70</v>
@@ -2456,13 +2466,13 @@
         <v>1.0000000000000001E-5</v>
       </c>
       <c r="K37" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
       <c r="L37" t="s">
         <v>22</v>
       </c>
       <c r="M37" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="N37">
         <v>60716271</v>
@@ -2476,7 +2486,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
       <c r="B38" t="s">
         <v>34</v>
@@ -2512,7 +2522,7 @@
         <v>22</v>
       </c>
       <c r="M38" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
       <c r="N38">
         <v>55936239</v>
@@ -2526,7 +2536,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
       <c r="B39" t="s">
         <v>34</v>
@@ -2562,7 +2572,7 @@
         <v>22</v>
       </c>
       <c r="M39" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
       <c r="N39">
         <v>55936239</v>
@@ -2576,7 +2586,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
       <c r="B40" t="s">
         <v>34</v>
@@ -2626,7 +2636,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B41" t="s">
         <v>34</v>
@@ -2726,7 +2736,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
-        <v>94</v>
+        <v>105</v>
       </c>
       <c r="B43" t="s">
         <v>34</v>
@@ -2822,6 +2832,106 @@
       </c>
       <c r="P44">
         <v>2300.2828860282898</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>109</v>
+      </c>
+      <c r="B45" t="s">
+        <v>34</v>
+      </c>
+      <c r="C45">
+        <v>0.95711892797319931</v>
+      </c>
+      <c r="D45">
+        <v>0.91600000000000004</v>
+      </c>
+      <c r="E45">
+        <v>7</v>
+      </c>
+      <c r="F45" t="s">
+        <v>95</v>
+      </c>
+      <c r="G45" t="s">
+        <v>61</v>
+      </c>
+      <c r="H45" t="s">
+        <v>62</v>
+      </c>
+      <c r="I45">
+        <v>100</v>
+      </c>
+      <c r="J45">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K45" t="s">
+        <v>110</v>
+      </c>
+      <c r="L45" t="s">
+        <v>22</v>
+      </c>
+      <c r="M45" t="s">
+        <v>91</v>
+      </c>
+      <c r="N45">
+        <v>55936239</v>
+      </c>
+      <c r="O45">
+        <v>0</v>
+      </c>
+      <c r="P45">
+        <v>6391.827333688736</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>111</v>
+      </c>
+      <c r="B46" t="s">
+        <v>34</v>
+      </c>
+      <c r="C46">
+        <v>0.97185929648241209</v>
+      </c>
+      <c r="D46">
+        <v>0.92333333333333334</v>
+      </c>
+      <c r="E46">
+        <v>7</v>
+      </c>
+      <c r="F46" t="s">
+        <v>95</v>
+      </c>
+      <c r="G46" t="s">
+        <v>61</v>
+      </c>
+      <c r="H46" t="s">
+        <v>62</v>
+      </c>
+      <c r="I46">
+        <v>200</v>
+      </c>
+      <c r="J46">
+        <v>1.0000000000000001E-5</v>
+      </c>
+      <c r="K46" t="s">
+        <v>112</v>
+      </c>
+      <c r="L46" t="s">
+        <v>22</v>
+      </c>
+      <c r="M46" t="s">
+        <v>91</v>
+      </c>
+      <c r="N46">
+        <v>55936239</v>
+      </c>
+      <c r="O46">
+        <v>0</v>
+      </c>
+      <c r="P46">
+        <v>8905.7663018703461</v>
       </c>
     </row>
   </sheetData>

</xml_diff>